<commit_message>
add: btap tuan 05
</commit_message>
<xml_diff>
--- a/Module02/DuongThaiBao_Module02.xlsx
+++ b/Module02/DuongThaiBao_Module02.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Bài 01" sheetId="1" r:id="rId1"/>
@@ -1130,6 +1130,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1166,12 +1183,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1187,17 +1210,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1217,20 +1252,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1277,41 +1312,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2300,16 +2300,16 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="90" t="s">
+      <c r="A21" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="91"/>
-      <c r="G21" s="91"/>
-      <c r="H21" s="91"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -2318,12 +2318,12 @@
       <c r="B22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
       <c r="G22" s="38" t="s">
         <v>207</v>
       </c>
@@ -2332,79 +2332,79 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="53"/>
+      <c r="A24" s="63"/>
       <c r="B24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="53"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="48" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C27" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="96" t="s">
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="43" t="s">
         <v>225</v>
       </c>
       <c r="H27" s="5">
@@ -2412,17 +2412,17 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="41"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="97" t="s">
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="44" t="s">
         <v>226</v>
       </c>
       <c r="H28" s="2">
@@ -2430,47 +2430,47 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="41"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="97" t="s">
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="44" t="s">
         <v>227</v>
       </c>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="41"/>
+      <c r="A30" s="48"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="97" t="s">
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="44" t="s">
         <v>228</v>
       </c>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="98" t="s">
+      <c r="A31" s="60" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="43" t="s">
+      <c r="C31" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="97" t="s">
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="44" t="s">
         <v>229</v>
       </c>
       <c r="H31" s="2">
@@ -2478,17 +2478,17 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="99"/>
+      <c r="A32" s="61"/>
       <c r="B32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="97" t="s">
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="44" t="s">
         <v>234</v>
       </c>
       <c r="H32" s="2">
@@ -2496,55 +2496,55 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="99"/>
+      <c r="A33" s="61"/>
       <c r="B33" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="43" t="s">
+      <c r="C33" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="97" t="s">
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="44" t="s">
         <v>230</v>
       </c>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="99"/>
+      <c r="A34" s="61"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="43" t="s">
+      <c r="C34" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="97" t="s">
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="44" t="s">
         <v>231</v>
       </c>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="99"/>
+      <c r="A35" s="61"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="97" t="s">
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="44" t="s">
         <v>232</v>
       </c>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="99"/>
+      <c r="A36" s="61"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="97" t="s">
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="44" t="s">
         <v>233</v>
       </c>
       <c r="H36" s="2"/>
@@ -2556,36 +2556,36 @@
       <c r="F37" s="12"/>
     </row>
     <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="48"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="55"/>
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="44" t="s">
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="51" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="8" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="45"/>
-      <c r="B40" s="45"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="52"/>
       <c r="C40" s="6" t="s">
         <v>5</v>
       </c>
@@ -2598,10 +2598,10 @@
       <c r="F40" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G40" s="45"/>
+      <c r="G40" s="52"/>
     </row>
     <row r="41" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="49" t="s">
         <v>84</v>
       </c>
       <c r="B41" s="5">
@@ -2624,7 +2624,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="52"/>
+      <c r="A42" s="59"/>
       <c r="B42" s="5">
         <v>2</v>
       </c>
@@ -2645,7 +2645,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="52"/>
+      <c r="A43" s="59"/>
       <c r="B43" s="5">
         <v>3</v>
       </c>
@@ -2666,7 +2666,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="48" t="s">
         <v>85</v>
       </c>
       <c r="B44" s="5">
@@ -2689,7 +2689,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="41"/>
+      <c r="A45" s="48"/>
       <c r="B45" s="5">
         <v>2</v>
       </c>
@@ -2708,7 +2708,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="41"/>
+      <c r="A46" s="48"/>
       <c r="B46" s="5">
         <v>3</v>
       </c>
@@ -2729,7 +2729,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="41"/>
+      <c r="A47" s="48"/>
       <c r="B47" s="5">
         <v>4</v>
       </c>
@@ -2748,7 +2748,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="41"/>
+      <c r="A48" s="48"/>
       <c r="B48" s="5">
         <v>5</v>
       </c>
@@ -2769,7 +2769,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="41"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="5">
         <v>6</v>
       </c>
@@ -2790,7 +2790,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A50" s="41"/>
+      <c r="A50" s="48"/>
       <c r="B50" s="5">
         <v>7</v>
       </c>
@@ -2811,7 +2811,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="41"/>
+      <c r="A51" s="48"/>
       <c r="B51" s="5">
         <v>8</v>
       </c>
@@ -2830,7 +2830,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="41"/>
+      <c r="A52" s="48"/>
       <c r="B52" s="5">
         <v>9</v>
       </c>
@@ -2851,7 +2851,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="41"/>
+      <c r="A53" s="48"/>
       <c r="B53" s="5">
         <v>10</v>
       </c>
@@ -2872,7 +2872,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="41"/>
+      <c r="A54" s="48"/>
       <c r="B54" s="5">
         <v>11</v>
       </c>
@@ -2893,7 +2893,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="42"/>
+      <c r="A55" s="49"/>
       <c r="B55" s="5">
         <v>12</v>
       </c>
@@ -2912,7 +2912,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="42" t="s">
+      <c r="A56" s="49" t="s">
         <v>222</v>
       </c>
       <c r="B56" s="5">
@@ -2935,7 +2935,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="52"/>
+      <c r="A57" s="59"/>
       <c r="B57" s="5">
         <v>2</v>
       </c>
@@ -2956,7 +2956,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="52"/>
+      <c r="A58" s="59"/>
       <c r="B58" s="5">
         <v>3</v>
       </c>
@@ -2977,7 +2977,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="52"/>
+      <c r="A59" s="59"/>
       <c r="B59" s="5">
         <v>4</v>
       </c>
@@ -2998,7 +2998,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="52"/>
+      <c r="A60" s="59"/>
       <c r="B60" s="5">
         <v>5</v>
       </c>
@@ -3019,7 +3019,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="53"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="5">
         <v>6</v>
       </c>
@@ -3040,7 +3040,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="42" t="s">
+      <c r="A62" s="49" t="s">
         <v>238</v>
       </c>
       <c r="B62" s="5">
@@ -3063,7 +3063,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="52"/>
+      <c r="A63" s="59"/>
       <c r="B63" s="5">
         <v>2</v>
       </c>
@@ -3084,7 +3084,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="52"/>
+      <c r="A64" s="59"/>
       <c r="B64" s="5">
         <v>3</v>
       </c>
@@ -3105,7 +3105,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="53"/>
+      <c r="A65" s="63"/>
       <c r="B65" s="5">
         <v>4</v>
       </c>
@@ -3132,11 +3132,10 @@
       <c r="A67" s="17"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="93"/>
+      <c r="A68" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A56:A61"/>
     <mergeCell ref="A62:A65"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="A23:A24"/>
@@ -3145,11 +3144,11 @@
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C22:F22"/>
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="C24:F24"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C26:F26"/>
+    <mergeCell ref="A56:A61"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A44:A55"/>
     <mergeCell ref="C34:F34"/>
@@ -3165,6 +3164,7 @@
     <mergeCell ref="C35:F35"/>
     <mergeCell ref="C36:F36"/>
     <mergeCell ref="A31:A36"/>
+    <mergeCell ref="C22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3201,21 +3201,21 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="95"/>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="95"/>
-      <c r="G15" s="70" t="s">
+      <c r="B15" s="87"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="G15" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
-      <c r="K15" s="70"/>
-      <c r="L15" s="70"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84"/>
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -3233,18 +3233,18 @@
       <c r="E16" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="G16" s="85" t="s">
+      <c r="G16" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="H16" s="85" t="s">
+      <c r="H16" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="I16" s="82" t="s">
+      <c r="I16" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="83"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="88" t="s">
+      <c r="J16" s="96"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="101" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3258,8 +3258,8 @@
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="G17" s="86"/>
-      <c r="H17" s="86"/>
+      <c r="G17" s="99"/>
+      <c r="H17" s="99"/>
       <c r="I17" s="24" t="s">
         <v>163</v>
       </c>
@@ -3269,7 +3269,7 @@
       <c r="K17" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="L17" s="89"/>
+      <c r="L17" s="102"/>
     </row>
     <row r="18" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
@@ -3281,7 +3281,7 @@
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="G18" s="72" t="s">
+      <c r="G18" s="75" t="s">
         <v>84</v>
       </c>
       <c r="H18" s="2">
@@ -3310,7 +3310,7 @@
       <c r="C19" s="37"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="G19" s="73"/>
+      <c r="G19" s="85"/>
       <c r="H19" s="2">
         <v>2</v>
       </c>
@@ -3328,7 +3328,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="49" t="s">
         <v>174</v>
       </c>
       <c r="B20" s="37" t="s">
@@ -3343,7 +3343,7 @@
       <c r="E20" s="5">
         <v>-1</v>
       </c>
-      <c r="G20" s="74"/>
+      <c r="G20" s="76"/>
       <c r="H20" s="2">
         <v>3</v>
       </c>
@@ -3361,7 +3361,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="53"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
         <v>172</v>
@@ -3372,7 +3372,7 @@
       <c r="E21" s="5">
         <v>-1</v>
       </c>
-      <c r="G21" s="59" t="s">
+      <c r="G21" s="68" t="s">
         <v>85</v>
       </c>
       <c r="H21" s="2">
@@ -3384,7 +3384,7 @@
       <c r="J21" s="2">
         <v>5</v>
       </c>
-      <c r="K21" s="102">
+      <c r="K21" s="45">
         <v>-1</v>
       </c>
       <c r="L21" s="2" t="s">
@@ -3392,7 +3392,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G22" s="72"/>
+      <c r="G22" s="75"/>
       <c r="H22" s="2">
         <v>2</v>
       </c>
@@ -3430,7 +3430,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G24" s="59" t="s">
+      <c r="G24" s="68" t="s">
         <v>238</v>
       </c>
       <c r="H24" s="2">
@@ -3442,7 +3442,7 @@
       <c r="J24" s="2">
         <v>5</v>
       </c>
-      <c r="K24" s="102">
+      <c r="K24" s="45">
         <v>-1</v>
       </c>
       <c r="L24" s="2" t="s">
@@ -3450,7 +3450,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G25" s="59"/>
+      <c r="G25" s="68"/>
       <c r="H25" s="2">
         <v>2</v>
       </c>
@@ -3469,8 +3469,6 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="G18:G20"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="A15:E15"/>
@@ -3479,6 +3477,8 @@
     <mergeCell ref="G15:L15"/>
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="L16:L17"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="G18:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3514,19 +3514,19 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="E15" s="70" t="s">
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="E15" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -3538,18 +3538,18 @@
       <c r="C16" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="85" t="s">
+      <c r="E16" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="F16" s="85" t="s">
+      <c r="F16" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="G16" s="82" t="s">
+      <c r="G16" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="83"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="88" t="s">
+      <c r="H16" s="96"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="101" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3561,8 +3561,8 @@
         <v>181</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
       <c r="G17" s="24" t="s">
         <v>179</v>
       </c>
@@ -3572,7 +3572,7 @@
       <c r="I17" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="J17" s="89"/>
+      <c r="J17" s="102"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
@@ -3582,7 +3582,7 @@
         <v>183</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="75" t="s">
         <v>84</v>
       </c>
       <c r="F18" s="2">
@@ -3601,7 +3601,7 @@
         <v>185</v>
       </c>
       <c r="C19" s="37"/>
-      <c r="E19" s="73"/>
+      <c r="E19" s="85"/>
       <c r="F19" s="2">
         <v>2</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>186</v>
       </c>
       <c r="C20" s="37"/>
-      <c r="E20" s="73"/>
+      <c r="E20" s="85"/>
       <c r="F20" s="2">
         <v>3</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>188</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="E21" s="73"/>
+      <c r="E21" s="85"/>
       <c r="F21" s="2">
         <v>4</v>
       </c>
@@ -3665,7 +3665,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E22" s="74"/>
+      <c r="E22" s="76"/>
       <c r="F22" s="2">
         <v>5</v>
       </c>
@@ -3727,17 +3727,17 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="E15" s="70" t="s">
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="E15" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84"/>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -3749,16 +3749,16 @@
       <c r="C16" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="85" t="s">
+      <c r="E16" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="F16" s="85" t="s">
+      <c r="F16" s="98" t="s">
         <v>102</v>
       </c>
       <c r="G16" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="88" t="s">
+      <c r="H16" s="101" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3772,12 +3772,12 @@
       <c r="C17" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
       <c r="G17" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="H17" s="89"/>
+      <c r="H17" s="102"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
@@ -3860,17 +3860,17 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="E15" s="70" t="s">
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="E15" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84"/>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -3882,41 +3882,41 @@
       <c r="C16" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="85" t="s">
+      <c r="E16" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="F16" s="85" t="s">
+      <c r="F16" s="98" t="s">
         <v>102</v>
       </c>
       <c r="G16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="88" t="s">
+      <c r="H16" s="101" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="49" t="s">
         <v>199</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>202</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
       <c r="G17" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="H17" s="89"/>
+      <c r="H17" s="102"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="53"/>
+      <c r="A18" s="63"/>
       <c r="B18" s="37" t="s">
         <v>203</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="75" t="s">
         <v>84</v>
       </c>
       <c r="F18" s="2">
@@ -3930,7 +3930,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E19" s="74"/>
+      <c r="E19" s="76"/>
       <c r="F19" s="2">
         <v>2</v>
       </c>
@@ -3995,16 +3995,16 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="62"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="63"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="71"/>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -4013,12 +4013,12 @@
       <c r="B26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
       <c r="G26" s="38" t="s">
         <v>207</v>
       </c>
@@ -4027,18 +4027,18 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="48" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C27" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
       <c r="G27" s="5" t="s">
         <v>209</v>
       </c>
@@ -4047,14 +4047,14 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="41"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
       <c r="G28" s="5" t="s">
         <v>210</v>
       </c>
@@ -4063,54 +4063,54 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="41"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="41"/>
+      <c r="A30" s="48"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="41"/>
+      <c r="A31" s="48"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="43" t="s">
+      <c r="C31" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="59" t="s">
+      <c r="A32" s="68" t="s">
         <v>46</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
       <c r="G32" s="5">
         <v>18</v>
       </c>
@@ -4119,14 +4119,14 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="59"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="43" t="s">
+      <c r="C33" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
       <c r="G33" s="5">
         <v>64</v>
       </c>
@@ -4135,82 +4135,82 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="59"/>
+      <c r="A34" s="68"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="43" t="s">
+      <c r="C34" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="59"/>
+      <c r="A35" s="68"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="55" t="s">
+      <c r="C35" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="57"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="59"/>
+      <c r="A36" s="68"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="43" t="s">
+      <c r="C36" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="59" t="s">
+      <c r="A37" s="68" t="s">
         <v>50</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="43" t="s">
+      <c r="C37" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="59"/>
+      <c r="A38" s="68"/>
       <c r="B38" s="5"/>
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="59" t="s">
+      <c r="A39" s="68" t="s">
         <v>52</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="43" t="s">
+      <c r="C39" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
       <c r="G39" s="5" t="s">
         <v>209</v>
       </c>
@@ -4219,98 +4219,98 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="59"/>
+      <c r="A40" s="68"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="55" t="s">
+      <c r="C40" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="57"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="65"/>
+      <c r="F40" s="66"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="59"/>
+      <c r="A41" s="68"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="43" t="s">
+      <c r="C41" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="59"/>
+      <c r="A42" s="68"/>
       <c r="B42" s="5"/>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="59"/>
+      <c r="A43" s="68"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="55" t="s">
+      <c r="C43" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="F43" s="57"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="66"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="59"/>
+      <c r="A44" s="68"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="43" t="s">
+      <c r="C44" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
     </row>
     <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
     </row>
     <row r="47" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="44" t="s">
+      <c r="B47" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="49" t="s">
+      <c r="C47" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="44" t="s">
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="51" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="45"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="52"/>
       <c r="C48" s="6" t="s">
         <v>54</v>
       </c>
@@ -4323,7 +4323,7 @@
       <c r="F48" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G48" s="45"/>
+      <c r="G48" s="52"/>
     </row>
     <row r="49" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
@@ -4349,7 +4349,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="49" t="s">
         <v>85</v>
       </c>
       <c r="B50" s="4">
@@ -4372,7 +4372,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="52"/>
+      <c r="A51" s="59"/>
       <c r="B51" s="4">
         <v>2</v>
       </c>
@@ -4393,7 +4393,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="52"/>
+      <c r="A52" s="59"/>
       <c r="B52" s="4">
         <v>3</v>
       </c>
@@ -4413,8 +4413,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="52"/>
+    <row r="53" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A53" s="59"/>
       <c r="B53" s="4">
         <v>4</v>
       </c>
@@ -4435,7 +4435,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="52"/>
+      <c r="A54" s="59"/>
       <c r="B54" s="4">
         <v>5</v>
       </c>
@@ -4454,7 +4454,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="52"/>
+      <c r="A55" s="59"/>
       <c r="B55" s="4">
         <v>6</v>
       </c>
@@ -4475,7 +4475,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="52"/>
+      <c r="A56" s="59"/>
       <c r="B56" s="4">
         <v>7</v>
       </c>
@@ -4496,7 +4496,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="52"/>
+      <c r="A57" s="59"/>
       <c r="B57" s="4">
         <v>8</v>
       </c>
@@ -4517,7 +4517,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="52"/>
+      <c r="A58" s="59"/>
       <c r="B58" s="4">
         <v>9</v>
       </c>
@@ -4537,8 +4537,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="52"/>
+    <row r="59" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="59"/>
       <c r="B59" s="4">
         <v>10</v>
       </c>
@@ -4557,7 +4557,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A60" s="52"/>
+      <c r="A60" s="59"/>
       <c r="B60" s="4">
         <v>11</v>
       </c>
@@ -4578,7 +4578,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="52"/>
+      <c r="A61" s="59"/>
       <c r="B61" s="4">
         <v>12</v>
       </c>
@@ -4597,7 +4597,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="52"/>
+      <c r="A62" s="59"/>
       <c r="B62" s="4">
         <v>13</v>
       </c>
@@ -4618,7 +4618,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="52"/>
+      <c r="A63" s="59"/>
       <c r="B63" s="4">
         <v>14</v>
       </c>
@@ -4639,7 +4639,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A64" s="52"/>
+      <c r="A64" s="59"/>
       <c r="B64" s="4">
         <v>15</v>
       </c>
@@ -4659,8 +4659,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="52"/>
+    <row r="65" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A65" s="59"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
         <v>55</v>
@@ -4679,7 +4679,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="53"/>
+      <c r="A66" s="63"/>
       <c r="B66" s="4">
         <v>16</v>
       </c>
@@ -4698,7 +4698,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="48" t="s">
         <v>222</v>
       </c>
       <c r="B67" s="4">
@@ -4721,7 +4721,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="41"/>
+      <c r="A68" s="48"/>
       <c r="B68" s="4">
         <v>2</v>
       </c>
@@ -4742,7 +4742,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="100" t="s">
+      <c r="A69" s="72" t="s">
         <v>222</v>
       </c>
       <c r="B69" s="4">
@@ -4765,7 +4765,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="101"/>
+      <c r="A70" s="73"/>
       <c r="B70" s="4">
         <v>2</v>
       </c>
@@ -4786,7 +4786,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="101"/>
+      <c r="A71" s="73"/>
       <c r="B71" s="4">
         <v>3</v>
       </c>
@@ -4807,7 +4807,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="101"/>
+      <c r="A72" s="73"/>
       <c r="B72" s="4">
         <v>4</v>
       </c>
@@ -4828,7 +4828,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="101"/>
+      <c r="A73" s="73"/>
       <c r="B73" s="4">
         <v>5</v>
       </c>
@@ -4849,7 +4849,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="101"/>
+      <c r="A74" s="73"/>
       <c r="B74" s="4">
         <v>6</v>
       </c>
@@ -5069,8 +5069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D34" sqref="A25:D34"/>
+    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5089,13 +5089,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -5115,7 +5115,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="48" t="s">
         <v>80</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -5132,7 +5132,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="41"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="5" t="s">
         <v>98</v>
       </c>
@@ -5147,37 +5147,37 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
     </row>
     <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="64" t="s">
+      <c r="A25" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="79" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="68" t="s">
+      <c r="D25" s="81" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="65"/>
-      <c r="B26" s="67"/>
+      <c r="A26" s="78"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="69"/>
+      <c r="D26" s="82"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="75" t="s">
         <v>84</v>
       </c>
       <c r="B27" s="2">
@@ -5191,7 +5191,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="74"/>
+      <c r="A28" s="76"/>
       <c r="B28" s="2">
         <v>2</v>
       </c>
@@ -5203,7 +5203,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="72" t="s">
+      <c r="A29" s="75" t="s">
         <v>85</v>
       </c>
       <c r="B29" s="2">
@@ -5217,7 +5217,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="74"/>
+      <c r="A30" s="76"/>
       <c r="B30" s="2">
         <v>2</v>
       </c>
@@ -5229,7 +5229,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="72" t="s">
+      <c r="A31" s="75" t="s">
         <v>222</v>
       </c>
       <c r="B31" s="2">
@@ -5239,11 +5239,11 @@
         <v>1</v>
       </c>
       <c r="D31" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="74"/>
+      <c r="A32" s="76"/>
       <c r="B32" s="2">
         <v>2</v>
       </c>
@@ -5255,7 +5255,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="72" t="s">
+      <c r="A33" s="75" t="s">
         <v>238</v>
       </c>
       <c r="B33" s="2">
@@ -5269,7 +5269,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="74"/>
+      <c r="A34" s="76"/>
       <c r="B34" s="2">
         <v>2</v>
       </c>
@@ -5282,7 +5282,6 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A25:A26"/>
@@ -5292,6 +5291,7 @@
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5303,7 +5303,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5325,19 +5325,19 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="95"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="G24" s="70" t="s">
+      <c r="B24" s="87"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="G24" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="70"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="84"/>
+      <c r="J24" s="84"/>
     </row>
     <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
@@ -5355,21 +5355,21 @@
       <c r="E25" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="G25" s="71" t="s">
+      <c r="G25" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="71" t="s">
+      <c r="H25" s="83" t="s">
         <v>102</v>
       </c>
       <c r="I25" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="71" t="s">
+      <c r="J25" s="83" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="59" t="s">
+      <c r="A26" s="68" t="s">
         <v>104</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -5384,22 +5384,22 @@
       <c r="E26" s="5">
         <v>1581</v>
       </c>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="83"/>
       <c r="I26" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="J26" s="71"/>
+      <c r="J26" s="83"/>
     </row>
     <row r="27" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="59"/>
+      <c r="A27" s="68"/>
       <c r="B27" s="4" t="s">
         <v>150</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="G27" s="72" t="s">
+      <c r="G27" s="75" t="s">
         <v>105</v>
       </c>
       <c r="H27" s="2">
@@ -5413,26 +5413,26 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="59"/>
+      <c r="A28" s="68"/>
       <c r="B28" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-      <c r="G28" s="73"/>
+      <c r="G28" s="85"/>
       <c r="H28" s="2">
         <v>2</v>
       </c>
       <c r="I28" s="2">
-        <v>2023</v>
+        <v>2004</v>
       </c>
       <c r="J28" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G29" s="74"/>
+      <c r="G29" s="76"/>
       <c r="H29" s="2">
         <v>3</v>
       </c>
@@ -5526,19 +5526,19 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="94" t="s">
+      <c r="A16" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="95"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="G16" s="70" t="s">
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="G16" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="70"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="70"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
@@ -5556,16 +5556,16 @@
       <c r="E17" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="G17" s="71" t="s">
+      <c r="G17" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="71" t="s">
+      <c r="H17" s="83" t="s">
         <v>102</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="71" t="s">
+      <c r="J17" s="83" t="s">
         <v>108</v>
       </c>
     </row>
@@ -5581,12 +5581,12 @@
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="83"/>
       <c r="I18" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="J18" s="71"/>
+      <c r="J18" s="83"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G19" s="2" t="s">
@@ -5657,21 +5657,21 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="94" t="s">
+      <c r="A18" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="95"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="95"/>
-      <c r="E18" s="95"/>
-      <c r="G18" s="79" t="s">
+      <c r="B18" s="87"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="G18" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="81"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="94"/>
     </row>
     <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
@@ -5689,18 +5689,18 @@
       <c r="E19" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="G19" s="71" t="s">
+      <c r="G19" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="71" t="s">
+      <c r="H19" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="I19" s="82" t="s">
+      <c r="I19" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="83"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="71" t="s">
+      <c r="J19" s="96"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="83" t="s">
         <v>110</v>
       </c>
     </row>
@@ -5714,8 +5714,8 @@
       <c r="C20" s="2"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="83"/>
       <c r="I20" s="24" t="s">
         <v>113</v>
       </c>
@@ -5725,7 +5725,7 @@
       <c r="K20" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L20" s="71"/>
+      <c r="L20" s="83"/>
     </row>
     <row r="21" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -5737,7 +5737,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="G21" s="75" t="s">
+      <c r="G21" s="88" t="s">
         <v>84</v>
       </c>
       <c r="H21" s="2">
@@ -5766,7 +5766,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="G22" s="76"/>
+      <c r="G22" s="89"/>
       <c r="H22" s="2">
         <v>2</v>
       </c>
@@ -5784,7 +5784,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="59" t="s">
+      <c r="A23" s="68" t="s">
         <v>156</v>
       </c>
       <c r="B23" s="2"/>
@@ -5793,7 +5793,7 @@
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="G23" s="77"/>
+      <c r="G23" s="90"/>
       <c r="H23" s="2">
         <v>3</v>
       </c>
@@ -5811,14 +5811,14 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="59"/>
+      <c r="A24" s="68"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="G24" s="78" t="s">
+      <c r="G24" s="91" t="s">
         <v>85</v>
       </c>
       <c r="H24" s="2">
@@ -5836,14 +5836,14 @@
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="59"/>
+      <c r="A25" s="68"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
         <v>119</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="G25" s="78"/>
+      <c r="G25" s="91"/>
       <c r="H25" s="2">
         <v>2</v>
       </c>
@@ -5859,7 +5859,7 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="59"/>
+      <c r="A26" s="68"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
         <v>120</v>
@@ -5870,7 +5870,7 @@
       <c r="E26" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G26" s="78"/>
+      <c r="G26" s="91"/>
       <c r="H26" s="2">
         <v>3</v>
       </c>
@@ -5886,7 +5886,7 @@
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="59"/>
+      <c r="A27" s="68"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
         <v>121</v>
@@ -5897,7 +5897,7 @@
       <c r="E27" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="G27" s="78"/>
+      <c r="G27" s="91"/>
       <c r="H27" s="2">
         <v>4</v>
       </c>
@@ -5913,7 +5913,7 @@
       <c r="L27" s="2"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="59"/>
+      <c r="A28" s="68"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>122</v>
@@ -5924,7 +5924,7 @@
       <c r="E28" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="G28" s="78"/>
+      <c r="G28" s="91"/>
       <c r="H28" s="2">
         <v>5</v>
       </c>
@@ -5940,7 +5940,7 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G29" s="78"/>
+      <c r="G29" s="91"/>
       <c r="H29" s="2">
         <v>6</v>
       </c>
@@ -5957,6 +5957,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A18:E18"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="G24:G29"/>
     <mergeCell ref="G18:L18"/>
@@ -5964,8 +5966,6 @@
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="L19:L20"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6000,19 +6000,19 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
-      <c r="E17" s="79" t="s">
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="E17" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="81"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="94"/>
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
@@ -6024,18 +6024,18 @@
       <c r="C18" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="85" t="s">
+      <c r="E18" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="F18" s="85" t="s">
+      <c r="F18" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="G18" s="82" t="s">
+      <c r="G18" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="83"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="85" t="s">
+      <c r="H18" s="96"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="98" t="s">
         <v>110</v>
       </c>
     </row>
@@ -6047,8 +6047,8 @@
         <v>125</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
+      <c r="E19" s="99"/>
+      <c r="F19" s="99"/>
       <c r="G19" s="24" t="s">
         <v>113</v>
       </c>
@@ -6058,7 +6058,7 @@
       <c r="I19" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="J19" s="86"/>
+      <c r="J19" s="99"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -6068,7 +6068,7 @@
         <v>157</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="E20" s="75" t="s">
+      <c r="E20" s="88" t="s">
         <v>84</v>
       </c>
       <c r="F20" s="2">
@@ -6095,7 +6095,7 @@
         <v>158</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="E21" s="76"/>
+      <c r="E21" s="89"/>
       <c r="F21" s="2">
         <v>2</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>159</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="E22" s="76"/>
+      <c r="E22" s="89"/>
       <c r="F22" s="2">
         <v>3</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>160</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="E23" s="76"/>
+      <c r="E23" s="89"/>
       <c r="F23" s="2">
         <v>4</v>
       </c>
@@ -6170,7 +6170,7 @@
       <c r="C24" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E24" s="77"/>
+      <c r="E24" s="90"/>
       <c r="F24" s="2">
         <v>5</v>
       </c>
@@ -6226,8 +6226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="D18:E19"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6243,27 +6243,81 @@
     <col min="12" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="13">
+        <v>1484</v>
+      </c>
+      <c r="E9" s="13">
+        <f>50*D9</f>
+        <v>74200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="13">
+        <v>1533</v>
+      </c>
+      <c r="E10" s="13">
+        <f>50*D10</f>
+        <v>76650</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="13">
+        <v>1786</v>
+      </c>
+      <c r="E11" s="13">
+        <f>100*D11</f>
+        <v>178600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="13">
+        <v>2242</v>
+      </c>
+      <c r="E12" s="13">
+        <f>100*D12</f>
+        <v>224200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="13">
+        <v>2503</v>
+      </c>
+      <c r="E13" s="13">
+        <f>100*D13</f>
+        <v>250300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="13">
+        <v>2587</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" ref="E10:E14" si="0">50*D14</f>
+        <v>129350</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="92"/>
-      <c r="G17" s="79" t="s">
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="G17" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="81"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="94"/>
     </row>
     <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
@@ -6281,17 +6335,17 @@
       <c r="E18" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="G18" s="85" t="s">
+      <c r="G18" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="H18" s="85" t="s">
+      <c r="H18" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="82" t="s">
+      <c r="I18" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="83"/>
-      <c r="K18" s="85" t="s">
+      <c r="J18" s="96"/>
+      <c r="K18" s="98" t="s">
         <v>110</v>
       </c>
     </row>
@@ -6305,15 +6359,15 @@
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="86"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="99"/>
       <c r="I19" s="24" t="s">
         <v>132</v>
       </c>
       <c r="J19" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="K19" s="86"/>
+      <c r="K19" s="99"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="s">
@@ -6325,7 +6379,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="G20" s="72" t="s">
+      <c r="G20" s="75" t="s">
         <v>84</v>
       </c>
       <c r="H20" s="2">
@@ -6353,7 +6407,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="G21" s="73"/>
+      <c r="G21" s="85"/>
       <c r="H21" s="2">
         <v>2</v>
       </c>
@@ -6361,12 +6415,12 @@
         <v>25</v>
       </c>
       <c r="J21" s="2">
-        <f xml:space="preserve"> I21 + 50</f>
-        <v>75</v>
+        <f xml:space="preserve"> I21 + 51</f>
+        <v>76</v>
       </c>
       <c r="K21" s="33">
-        <f>(J21-I21)*1533*1.1</f>
-        <v>84315</v>
+        <f>(E9+(J21-I21-50)*1533)*1.1</f>
+        <v>83306.3</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -6379,7 +6433,7 @@
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="G22" s="73"/>
+      <c r="G22" s="85"/>
       <c r="H22" s="2">
         <v>3</v>
       </c>
@@ -6387,12 +6441,12 @@
         <v>25</v>
       </c>
       <c r="J22" s="2">
-        <f>I22 + 150</f>
-        <v>175</v>
+        <f>I22 + 151</f>
+        <v>176</v>
       </c>
       <c r="K22" s="33">
-        <f>(J22-I22)*1786*1.1</f>
-        <v>294690</v>
+        <f>(SUM(E9:E10)+(J22-I22-100)*1786)*1.1</f>
+        <v>266129.60000000003</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -6405,7 +6459,7 @@
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="G23" s="73"/>
+      <c r="G23" s="85"/>
       <c r="H23" s="2">
         <v>4</v>
       </c>
@@ -6413,12 +6467,12 @@
         <v>25</v>
       </c>
       <c r="J23" s="2">
-        <f xml:space="preserve"> I23 + 250</f>
-        <v>275</v>
+        <f xml:space="preserve"> I23 + 251</f>
+        <v>276</v>
       </c>
       <c r="K23" s="33">
-        <f>(J23-I23)*2242*1.1</f>
-        <v>616550</v>
+        <f>(SUM(E9:E11)+((J23-I23-200)*2242)*1.1)</f>
+        <v>455226.2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -6431,7 +6485,7 @@
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="G24" s="73"/>
+      <c r="G24" s="85"/>
       <c r="H24" s="2">
         <v>5</v>
       </c>
@@ -6439,16 +6493,16 @@
         <v>25</v>
       </c>
       <c r="J24" s="2">
-        <f xml:space="preserve"> I24 + 350</f>
-        <v>375</v>
+        <f xml:space="preserve"> I24 + 351</f>
+        <v>376</v>
       </c>
       <c r="K24" s="33">
-        <f>(J24-I24)*2503*1.1</f>
-        <v>963655.00000000012</v>
+        <f>(SUM(E9:E12)+(J24-I24-300)*2503)*1.1</f>
+        <v>749433.3</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="78" t="s">
+      <c r="A25" s="91" t="s">
         <v>161</v>
       </c>
       <c r="B25" s="2"/>
@@ -6461,7 +6515,7 @@
       <c r="E25" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="G25" s="73"/>
+      <c r="G25" s="85"/>
       <c r="H25" s="2">
         <v>6</v>
       </c>
@@ -6473,12 +6527,12 @@
         <v>525</v>
       </c>
       <c r="K25" s="33">
-        <f>(J25-I25)*2587</f>
-        <v>1293500</v>
+        <f>(SUM(E9:E13)+(J25-I25-400)*2587)*1.1</f>
+        <v>1168915</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="78"/>
+      <c r="A26" s="91"/>
       <c r="B26" s="2"/>
       <c r="C26" s="4" t="s">
         <v>135</v>
@@ -6489,7 +6543,7 @@
       <c r="E26" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="G26" s="72" t="s">
+      <c r="G26" s="75" t="s">
         <v>84</v>
       </c>
       <c r="H26" s="2">
@@ -6506,14 +6560,14 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="78"/>
+      <c r="A27" s="91"/>
       <c r="B27" s="2"/>
       <c r="C27" s="4" t="s">
         <v>134</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="G27" s="73"/>
+      <c r="G27" s="85"/>
       <c r="H27" s="2">
         <v>2</v>
       </c>
@@ -6528,7 +6582,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G28" s="74"/>
+      <c r="G28" s="76"/>
       <c r="H28" s="2">
         <v>3</v>
       </c>
@@ -6543,7 +6597,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G29" s="72" t="s">
+      <c r="G29" s="75" t="s">
         <v>222</v>
       </c>
       <c r="H29" s="2">
@@ -6562,7 +6616,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G30" s="74"/>
+      <c r="G30" s="76"/>
       <c r="H30" s="2">
         <v>2</v>
       </c>
@@ -6578,7 +6632,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G31" s="72" t="s">
+      <c r="G31" s="75" t="s">
         <v>238</v>
       </c>
       <c r="H31" s="2">
@@ -6595,7 +6649,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G32" s="74"/>
+      <c r="G32" s="76"/>
       <c r="H32" s="2">
         <v>2</v>
       </c>
@@ -6661,18 +6715,18 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="E15" s="79" t="s">
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="E15" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="81"/>
+      <c r="F15" s="93"/>
+      <c r="G15" s="93"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="94"/>
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -6684,30 +6738,30 @@
       <c r="C16" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="85" t="s">
+      <c r="E16" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="F16" s="85" t="s">
+      <c r="F16" s="98" t="s">
         <v>102</v>
       </c>
       <c r="G16" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="87" t="s">
+      <c r="H16" s="100" t="s">
         <v>110</v>
       </c>
-      <c r="I16" s="87"/>
+      <c r="I16" s="100"/>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="68" t="s">
         <v>162</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>204</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
       <c r="G17" s="24" t="s">
         <v>162</v>
       </c>
@@ -6719,12 +6773,12 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="59"/>
+      <c r="A18" s="68"/>
       <c r="B18" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="75" t="s">
         <v>84</v>
       </c>
       <c r="F18" s="2">
@@ -6741,7 +6795,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E19" s="73"/>
+      <c r="E19" s="85"/>
       <c r="F19" s="2">
         <v>2</v>
       </c>

</xml_diff>